<commit_message>
Updated test submit custom order as admin
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageProfile.xlsx
+++ b/binaries/FCfiles/ManageProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129075DF-7631-457D-8CDB-212358053D34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B51401A-E7B2-49DF-9933-5A100C18BA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FF125F1C-9927-44E3-BE4C-8ED054D4B06E}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>Carrier</t>
   </si>
   <si>
-    <t>BTX Global Logistics, Ceva,ABF Freight,FC Test Carrier</t>
+    <t>ABF Freight, BTX Global Logistics, Ceva,FC Test Carrier, Ups</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Updated UPS carrier name in data file
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageProfile.xlsx
+++ b/binaries/FCfiles/ManageProfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B51401A-E7B2-49DF-9933-5A100C18BA04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02425D8E-47AF-4580-B9B8-85DDCB65058D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FF125F1C-9927-44E3-BE4C-8ED054D4B06E}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>Carrier</t>
   </si>
   <si>
-    <t>ABF Freight, BTX Global Logistics, Ceva,FC Test Carrier, Ups</t>
+    <t>ABF Freight, BTX Global Logistics, Ceva,FC Test Carrier, UPS</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>